<commit_message>
Jobsheet 8 - tugas 3
</commit_message>
<xml_diff>
--- a/public/template_user.xlsx
+++ b/public/template_user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester_4\PemrogramanWeb\laragon\www\PWL_POS\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACDDC71-5F45-4828-B384-88D24F7C0F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1898A33-3CE0-45F7-A064-BAB0E7733593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02442A19-32FB-4827-93ED-F030B6ECAF78}"/>
+    <workbookView xWindow="910" yWindow="340" windowWidth="14400" windowHeight="7270" xr2:uid="{02442A19-32FB-4827-93ED-F030B6ECAF78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -45,16 +45,19 @@
     <t>level_id</t>
   </si>
   <si>
+    <t>Salma</t>
+  </si>
+  <si>
+    <t>Staff Barang</t>
+  </si>
+  <si>
     <t>password</t>
   </si>
   <si>
-    <t>Salma</t>
-  </si>
-  <si>
-    <t>Staff Barang</t>
-  </si>
-  <si>
-    <t>staffbarang</t>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Nadira</t>
   </si>
 </sst>
 </file>
@@ -415,19 +418,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28465CA-5C15-4591-9CFD-DBE0DDF13532}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -438,21 +441,35 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>